<commit_message>
Changed algorithm and conditional formatting for the AiBi acceptor.
</commit_message>
<xml_diff>
--- a/stateTableReferencing.xlsx
+++ b/stateTableReferencing.xlsx
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,31 +780,31 @@
         <v>$A$22:$C$22</v>
       </c>
       <c r="C17" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",C17)-1-transition_table_row1))+(CELL("col",C17)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",C17))+((transition_table_width)*(CELL("row",C17)-1-transition_table_row1))+(CELL("col",C17)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ref="B17:I21" ca="1" si="0">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",C17)-1-transition_table_row1))+(CELL("col",C17)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",C17))+((transition_table_width)*(CELL("row",C17)-1-transition_table_row1))+(CELL("col",C17)-transition_table_col1)+transition_table_height-1,3))</f>
         <v>$A$23:$C$23</v>
       </c>
       <c r="D17" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",D17)-1-transition_table_row1))+(CELL("col",D17)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",D17))+((transition_table_width)*(CELL("row",D17)-1-transition_table_row1))+(CELL("col",D17)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$24:$C$24</v>
       </c>
       <c r="E17" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",E17)-1-transition_table_row1))+(CELL("col",E17)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",E17))+((transition_table_width)*(CELL("row",E17)-1-transition_table_row1))+(CELL("col",E17)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$25:$C$25</v>
       </c>
       <c r="F17" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",F17)-1-transition_table_row1))+(CELL("col",F17)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",F17))+((transition_table_width)*(CELL("row",F17)-1-transition_table_row1))+(CELL("col",F17)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$26:$C$26</v>
       </c>
       <c r="G17" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",G17)-1-transition_table_row1))+(CELL("col",G17)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",G17))+((transition_table_width)*(CELL("row",G17)-1-transition_table_row1))+(CELL("col",G17)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$27:$C$27</v>
       </c>
       <c r="H17" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",H17)-1-transition_table_row1))+(CELL("col",H17)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",H17))+((transition_table_width)*(CELL("row",H17)-1-transition_table_row1))+(CELL("col",H17)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$28:$C$28</v>
       </c>
       <c r="I17" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",I17)-1-transition_table_row1))+(CELL("col",I17)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",I17))+((transition_table_width)*(CELL("row",I17)-1-transition_table_row1))+(CELL("col",I17)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$29:$C$29</v>
       </c>
     </row>
@@ -813,35 +813,35 @@
         <v>11</v>
       </c>
       <c r="B18" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",B18)-1-transition_table_row1))+(CELL("col",B18)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",B18))+((transition_table_width)*(CELL("row",B18)-1-transition_table_row1))+(CELL("col",B18)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$30:$C$31</v>
       </c>
       <c r="C18" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",C18)-1-transition_table_row1))+(CELL("col",C18)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",C18))+((transition_table_width)*(CELL("row",C18)-1-transition_table_row1))+(CELL("col",C18)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$31:$C$32</v>
       </c>
       <c r="D18" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",D18)-1-transition_table_row1))+(CELL("col",D18)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",D18))+((transition_table_width)*(CELL("row",D18)-1-transition_table_row1))+(CELL("col",D18)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$32:$C$33</v>
       </c>
       <c r="E18" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",E18)-1-transition_table_row1))+(CELL("col",E18)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",E18))+((transition_table_width)*(CELL("row",E18)-1-transition_table_row1))+(CELL("col",E18)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$33:$C$34</v>
       </c>
       <c r="F18" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",F18)-1-transition_table_row1))+(CELL("col",F18)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",F18))+((transition_table_width)*(CELL("row",F18)-1-transition_table_row1))+(CELL("col",F18)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$34:$C$35</v>
       </c>
       <c r="G18" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",G18)-1-transition_table_row1))+(CELL("col",G18)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",G18))+((transition_table_width)*(CELL("row",G18)-1-transition_table_row1))+(CELL("col",G18)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$35:$C$36</v>
       </c>
       <c r="H18" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",H18)-1-transition_table_row1))+(CELL("col",H18)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",H18))+((transition_table_width)*(CELL("row",H18)-1-transition_table_row1))+(CELL("col",H18)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$36:$C$37</v>
       </c>
       <c r="I18" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",I18)-1-transition_table_row1))+(CELL("col",I18)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",I18))+((transition_table_width)*(CELL("row",I18)-1-transition_table_row1))+(CELL("col",I18)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$37:$C$38</v>
       </c>
     </row>
@@ -850,35 +850,35 @@
         <v>12</v>
       </c>
       <c r="B19" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",B19)-1-transition_table_row1))+(CELL("col",B19)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",B19))+((transition_table_width)*(CELL("row",B19)-1-transition_table_row1))+(CELL("col",B19)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$38:$C$40</v>
       </c>
       <c r="C19" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",C19)-1-transition_table_row1))+(CELL("col",C19)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",C19))+((transition_table_width)*(CELL("row",C19)-1-transition_table_row1))+(CELL("col",C19)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$39:$C$41</v>
       </c>
       <c r="D19" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",D19)-1-transition_table_row1))+(CELL("col",D19)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",D19))+((transition_table_width)*(CELL("row",D19)-1-transition_table_row1))+(CELL("col",D19)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$40:$C$42</v>
       </c>
       <c r="E19" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",E19)-1-transition_table_row1))+(CELL("col",E19)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",E19))+((transition_table_width)*(CELL("row",E19)-1-transition_table_row1))+(CELL("col",E19)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$41:$C$43</v>
       </c>
       <c r="F19" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",F19)-1-transition_table_row1))+(CELL("col",F19)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",F19))+((transition_table_width)*(CELL("row",F19)-1-transition_table_row1))+(CELL("col",F19)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$42:$C$44</v>
       </c>
       <c r="G19" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",G19)-1-transition_table_row1))+(CELL("col",G19)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",G19))+((transition_table_width)*(CELL("row",G19)-1-transition_table_row1))+(CELL("col",G19)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$43:$C$45</v>
       </c>
       <c r="H19" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",H19)-1-transition_table_row1))+(CELL("col",H19)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",H19))+((transition_table_width)*(CELL("row",H19)-1-transition_table_row1))+(CELL("col",H19)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$44:$C$46</v>
       </c>
       <c r="I19" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",I19)-1-transition_table_row1))+(CELL("col",I19)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",I19))+((transition_table_width)*(CELL("row",I19)-1-transition_table_row1))+(CELL("col",I19)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$45:$C$47</v>
       </c>
     </row>
@@ -887,69 +887,69 @@
         <v>13</v>
       </c>
       <c r="B20" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",B20)-1-transition_table_row1))+(CELL("col",B20)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",B20))+((transition_table_width)*(CELL("row",B20)-1-transition_table_row1))+(CELL("col",B20)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$46:$C$49</v>
       </c>
       <c r="C20" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",C20)-1-transition_table_row1))+(CELL("col",C20)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",C20))+((transition_table_width)*(CELL("row",C20)-1-transition_table_row1))+(CELL("col",C20)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$47:$C$50</v>
       </c>
       <c r="D20" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",D20)-1-transition_table_row1))+(CELL("col",D20)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",D20))+((transition_table_width)*(CELL("row",D20)-1-transition_table_row1))+(CELL("col",D20)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$48:$C$51</v>
       </c>
       <c r="E20" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",E20)-1-transition_table_row1))+(CELL("col",E20)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",E20))+((transition_table_width)*(CELL("row",E20)-1-transition_table_row1))+(CELL("col",E20)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$49:$C$52</v>
       </c>
       <c r="F20" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",F20)-1-transition_table_row1))+(CELL("col",F20)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",F20))+((transition_table_width)*(CELL("row",F20)-1-transition_table_row1))+(CELL("col",F20)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$50:$C$53</v>
       </c>
       <c r="G20" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",G20)-1-transition_table_row1))+(CELL("col",G20)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",G20))+((transition_table_width)*(CELL("row",G20)-1-transition_table_row1))+(CELL("col",G20)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$51:$C$54</v>
       </c>
       <c r="H20" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",H20)-1-transition_table_row1))+(CELL("col",H20)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",H20))+((transition_table_width)*(CELL("row",H20)-1-transition_table_row1))+(CELL("col",H20)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$52:$C$55</v>
       </c>
       <c r="I20" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",I20)-1-transition_table_row1))+(CELL("col",I20)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",I20))+((transition_table_width)*(CELL("row",I20)-1-transition_table_row1))+(CELL("col",I20)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$53:$C$56</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",B21)-1-transition_table_row1))+(CELL("col",B21)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",B21))+((transition_table_width)*(CELL("row",B21)-1-transition_table_row1))+(CELL("col",B21)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$54:$C$58</v>
       </c>
       <c r="C21" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",C21)-1-transition_table_row1))+(CELL("col",C21)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",C21))+((transition_table_width)*(CELL("row",C21)-1-transition_table_row1))+(CELL("col",C21)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$55:$C$59</v>
       </c>
       <c r="D21" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",D21)-1-transition_table_row1))+(CELL("col",D21)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",D21))+((transition_table_width)*(CELL("row",D21)-1-transition_table_row1))+(CELL("col",D21)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$56:$C$60</v>
       </c>
       <c r="E21" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",E21)-1-transition_table_row1))+(CELL("col",E21)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",E21))+((transition_table_width)*(CELL("row",E21)-1-transition_table_row1))+(CELL("col",E21)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$57:$C$61</v>
       </c>
       <c r="F21" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",F21)-1-transition_table_row1))+(CELL("col",F21)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",F21))+((transition_table_width)*(CELL("row",F21)-1-transition_table_row1))+(CELL("col",F21)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$58:$C$62</v>
       </c>
       <c r="G21" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",G21)-1-transition_table_row1))+(CELL("col",G21)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",G21))+((transition_table_width)*(CELL("row",G21)-1-transition_table_row1))+(CELL("col",G21)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$59:$C$63</v>
       </c>
       <c r="H21" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",H21)-1-transition_table_row1))+(CELL("col",H21)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",H21))+((transition_table_width)*(CELL("row",H21)-1-transition_table_row1))+(CELL("col",H21)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$60:$C$64</v>
       </c>
       <c r="I21" t="str">
-        <f ca="1">CONCATENATE(ADDRESS(transition_table_row1+1+((transition_table_width)*(CELL("row",I21)-1-transition_table_row1))+(CELL("col",I21)-transition_table_col1)+transition_table_height-1,1),":",ADDRESS((CELL("row",I21))+((transition_table_width)*(CELL("row",I21)-1-transition_table_row1))+(CELL("col",I21)-transition_table_col1)+transition_table_height-1,3))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>$A$61:$C$65</v>
       </c>
     </row>

</xml_diff>